<commit_message>
takes data from form and populates corresponding cell in excel
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -35,7 +35,10 @@
     <t>txt1</t>
   </si>
   <si>
-    <t xml:space="preserve">aaron</t>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
   </si>
 </sst>
 </file>
@@ -371,6 +374,9 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated naming and js for multiple entries per row
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/AARON 128/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronrotem/Documents/FormSite/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,10 +35,22 @@
     <t>txt1</t>
   </si>
   <si>
+    <t>Total Number of Units</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
     <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">b</t>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
   </si>
 </sst>
 </file>
@@ -357,25 +369,39 @@
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>